<commit_message>
Finished Analysis on SSdata
</commit_message>
<xml_diff>
--- a/SSdata.xlsx
+++ b/SSdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley Kwan\Desktop\College Stuff\EE 514\EE514_Project\EE514_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B421CB-3616-4078-9549-E6668B3BC69C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B9D7C0-8A8E-4659-B426-5A0E13A304AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1290" yWindow="1440" windowWidth="21600" windowHeight="11835" xr2:uid="{CE68294A-8B46-A34F-B91F-F31125F43B14}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{CE68294A-8B46-A34F-B91F-F31125F43B14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -123,62 +123,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Finding Ka</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -199,16 +144,163 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.0476544977332379E-2"/>
+                  <c:y val="-0.58952263357825774"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="CMU Serif Extra" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                        <a:ea typeface="CMU Serif Extra" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                        <a:cs typeface="CMU Serif Extra" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                      </a:rPr>
+                      <a:t>y = -</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" i="0" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                        <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                        <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                      </a:rPr>
+                      <a:t>5.1793</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="CMU Serif Extra" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                        <a:ea typeface="CMU Serif Extra" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                        <a:cs typeface="CMU Serif Extra" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                      </a:rPr>
+                      <a:t>x</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" sz="1200" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="CMU Serif Extra" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                        <a:ea typeface="CMU Serif Extra" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                        <a:cs typeface="CMU Serif Extra" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                      </a:rPr>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="CMU Serif Extra" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                        <a:ea typeface="CMU Serif Extra" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                        <a:cs typeface="CMU Serif Extra" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                      </a:rPr>
+                      <a:t>R² = </a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                        <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                        <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                      </a:rPr>
+                      <a:t>0.9979</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1200">
+                      <a:solidFill>
+                        <a:sysClr val="windowText" lastClr="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                      <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                      <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    </a:endParaRPr>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$C$3:$C$13</c:f>
@@ -232,9 +324,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>-2.04</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.223</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>-0.46300000000000002</c:v>
@@ -274,9 +363,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>10.86</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.77400000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2.06</c:v>
@@ -318,32 +404,77 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  </a:rPr>
+                  <a:t>Power Amp Input [V]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -354,12 +485,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -377,35 +505,81 @@
         <c:axId val="884695519"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  </a:rPr>
+                  <a:t>Motor Voltage [V]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="high"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -416,12 +590,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -438,7 +609,9 @@
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -459,12 +632,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -482,7 +650,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1047,16 +1215,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>319087</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>276226</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>700087</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>485776</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1383,8 +1551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C3CE229-3C40-9E49-8365-2E171C647745}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1528,24 +1696,6 @@
         <v>-33</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0.223</v>
-      </c>
-      <c r="D9">
-        <v>0.77400000000000002</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>245</v>
@@ -1620,6 +1770,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished Sensor Gain Analysis
Found Km, Kt, tau_m. Additionally, created figures for the stated gains and values
</commit_message>
<xml_diff>
--- a/SSdata.xlsx
+++ b/SSdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley Kwan\Desktop\College Stuff\EE 514\EE514_Project\EE514_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B9D7C0-8A8E-4659-B426-5A0E13A304AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFE2EBE-D925-4ED0-AA93-6ACB41398AF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{CE68294A-8B46-A34F-B91F-F31125F43B14}"/>
+    <workbookView minimized="1" xWindow="-195" yWindow="3270" windowWidth="21600" windowHeight="11835" xr2:uid="{CE68294A-8B46-A34F-B91F-F31125F43B14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,13 +61,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="CMU Serif Extra"/>
     </font>
   </fonts>
   <fills count="2">
@@ -90,8 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,7 +522,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -529,7 +535,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400">
+                  <a:rPr lang="en-US" sz="1200">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -555,7 +561,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -655,7 +661,995 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.7428542020482735E-2"/>
+                  <c:y val="0.59459720764482638"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$3:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.86</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.06</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.56</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.067840827778852</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>94.247779607693786</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>151.84364492350667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>188.49555921538757</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>230.38346126325149</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25.656340004316643</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.660765716752367</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.2831853071795862</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AF16-435F-A342-03852D76FF3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="884698015"/>
+        <c:axId val="884695519"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="884698015"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  </a:rPr>
+                  <a:t>Motor Voltage [V]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="884695519"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="884695519"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  </a:rPr>
+                  <a:t>Motor</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  </a:rPr>
+                  <a:t> Speed </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  </a:rPr>
+                  <a:t>[rad/s]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="884698015"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.500150683324302E-2"/>
+                  <c:y val="-0.62052933686630762"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:sysClr val="windowText" lastClr="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="CMU Serif Extra" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                      <a:ea typeface="CMU Serif Extra" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                      <a:cs typeface="CMU Serif Extra" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.067840827778852</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>94.247779607693786</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>151.84364492350667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>188.49555921538757</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>230.38346126325149</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25.656340004316643</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.660765716752367</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.2831853071795862</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$3:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-13.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-21.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-27.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-3.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1.65</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A6C3-442E-999E-4560B65DFFC6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1271580880"/>
+        <c:axId val="1271579632"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1271580880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  </a:rPr>
+                  <a:t>Motor Speed [rad/s]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="high"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1271579632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1271579632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  </a:rPr>
+                  <a:t>Tachometer Voltage [V]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1271580880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1211,6 +2205,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1244,6 +3270,80 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C58E4409-862E-479D-8F27-52F9B4961C60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>361949</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>166686</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D3B5F14-8B41-437D-8A04-FC2799A43C27}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1549,10 +3649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C3CE229-3C40-9E49-8365-2E171C647745}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1768,6 +3868,9 @@
         <v>-1.01</v>
       </c>
     </row>
+    <row r="19" spans="15:15" ht="20.25" x14ac:dyDescent="0.4">
+      <c r="O19" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
slight updates to excel sheets
</commit_message>
<xml_diff>
--- a/SSdata.xlsx
+++ b/SSdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley Kwan\Desktop\College Stuff\EE 514\EE514_Project\EE514_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDCBFCC-6835-4F9E-ADC4-647B6305C58B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4CE248-18F2-432B-BA9A-DCAC3050850B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{CE68294A-8B46-A34F-B91F-F31125F43B14}"/>
+    <workbookView minimized="1" xWindow="6000" yWindow="5415" windowWidth="19185" windowHeight="10785" xr2:uid="{CE68294A-8B46-A34F-B91F-F31125F43B14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4800,7 +4800,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R30" sqref="R30"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5032,7 +5032,7 @@
         <v>-68.067840827778852</v>
       </c>
       <c r="D16">
-        <f t="shared" ref="C16:D25" si="2">D4*-1</f>
+        <f t="shared" ref="D16:D25" si="2">D4*-1</f>
         <v>-4.25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated open loop testing
</commit_message>
<xml_diff>
--- a/SSdata.xlsx
+++ b/SSdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley Kwan\Desktop\College Stuff\EE 514\EE514_Project\EE514_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4CE248-18F2-432B-BA9A-DCAC3050850B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC6BD47-49A7-40A0-ACC5-434D1A637C2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="6000" yWindow="5415" windowWidth="19185" windowHeight="10785" xr2:uid="{CE68294A-8B46-A34F-B91F-F31125F43B14}"/>
+    <workbookView xWindow="14520" yWindow="6105" windowWidth="19185" windowHeight="10785" xr2:uid="{CE68294A-8B46-A34F-B91F-F31125F43B14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Motor speed</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>[rad/s]</t>
+  </si>
+  <si>
+    <t>Rad</t>
   </si>
 </sst>
 </file>
@@ -331,6 +334,9 @@
                 <c:pt idx="5">
                   <c:v>-2.04</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.223</c:v>
+                </c:pt>
                 <c:pt idx="7">
                   <c:v>-0.46300000000000002</c:v>
                 </c:pt>
@@ -369,6 +375,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>10.86</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.77400000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2.06</c:v>
@@ -781,6 +790,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>10.86</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.77400000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2.06</c:v>
@@ -1688,6 +1700,9 @@
                 <c:pt idx="5">
                   <c:v>10.86</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.77400000000000002</c:v>
+                </c:pt>
                 <c:pt idx="7">
                   <c:v>2.06</c:v>
                 </c:pt>
@@ -1699,39 +1714,6 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1.3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.5000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-4.25</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-5.36</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-7.6</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-9.26</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-10.86</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-2.06</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-1.56</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-1.07</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-1.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1771,39 +1753,6 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>6.2831853071795862</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-68.067840827778852</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-94.247779607693786</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-151.84364492350667</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-188.49555921538757</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-230.38346126325149</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-25.656340004316643</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-14.660765716752367</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-6.2831853071795862</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4797,10 +4746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C3CE229-3C40-9E49-8365-2E171C647745}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4809,6 +4758,9 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
@@ -4944,6 +4896,14 @@
         <v>-33</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>-0.223</v>
+      </c>
+      <c r="D9">
+        <v>-0.77400000000000002</v>
+      </c>
+    </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>245</v>
@@ -5016,116 +4976,8 @@
         <v>-1.01</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <f>-1*B3</f>
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <f>D3*-1</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <f t="shared" ref="B16:B25" si="1">-1*B4</f>
-        <v>-68.067840827778852</v>
-      </c>
-      <c r="D16">
-        <f t="shared" ref="D16:D25" si="2">D4*-1</f>
-        <v>-4.25</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <f t="shared" si="1"/>
-        <v>-94.247779607693786</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="2"/>
-        <v>-5.36</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <f t="shared" si="1"/>
-        <v>-151.84364492350667</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="2"/>
-        <v>-7.6</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" ht="20.25" x14ac:dyDescent="0.4">
-      <c r="B19">
-        <f t="shared" si="1"/>
-        <v>-188.49555921538757</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="2"/>
-        <v>-9.26</v>
-      </c>
+    <row r="19" spans="15:15" ht="20.25" x14ac:dyDescent="0.4">
       <c r="O19" s="1"/>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <f t="shared" si="1"/>
-        <v>-230.38346126325149</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="2"/>
-        <v>-10.86</v>
-      </c>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <f t="shared" si="1"/>
-        <v>-25.656340004316643</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="2"/>
-        <v>-2.06</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23">
-        <f t="shared" si="1"/>
-        <v>-14.660765716752367</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="2"/>
-        <v>-1.56</v>
-      </c>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="2"/>
-        <v>-1.07</v>
-      </c>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25">
-        <f t="shared" si="1"/>
-        <v>-6.2831853071795862</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="2"/>
-        <v>-1.3</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>